<commit_message>
edit olom week 5
</commit_message>
<xml_diff>
--- a/week 5/علوم/Skale(V3.6).xlsx
+++ b/week 5/علوم/Skale(V3.6).xlsx
@@ -748,15 +748,6 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -768,6 +759,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1502,8 +1502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2064,7 +2064,7 @@
         <v>1</v>
       </c>
       <c r="I18" s="42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J18" s="42">
         <v>4</v>
@@ -2857,18 +2857,18 @@
       <c r="L44" s="3"/>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A45" s="50"/>
-      <c r="B45" s="51"/>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="51"/>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="51"/>
-      <c r="I45" s="51"/>
-      <c r="J45" s="51"/>
-      <c r="K45" s="51"/>
-      <c r="L45" s="52"/>
+      <c r="A45" s="55"/>
+      <c r="B45" s="56"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="56"/>
+      <c r="E45" s="56"/>
+      <c r="F45" s="56"/>
+      <c r="G45" s="56"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
+      <c r="J45" s="56"/>
+      <c r="K45" s="56"/>
+      <c r="L45" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3935,7 +3935,7 @@
       </c>
       <c r="I18" s="10">
         <f>IF(گوگل!I18=کلید!H$2,3,IF(گوگل!I18="",0,-1))</f>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="10">
         <f>IF(گوگل!J18=کلید!I$2,3,IF(گوگل!J18="",0,-1))</f>
@@ -3951,7 +3951,7 @@
       </c>
       <c r="M18" s="11">
         <f t="shared" si="0"/>
-        <v>73.333333333333329</v>
+        <v>86.666666666666671</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="18.600000000000001" x14ac:dyDescent="0.25">
@@ -6375,7 +6375,7 @@
     <row r="3" spans="1:15" ht="18.600000000000001" x14ac:dyDescent="0.6">
       <c r="A3" s="24">
         <f t="shared" ref="A3:A42" si="0">RANK(O3, O$2:O$42)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>14</v>
@@ -6413,7 +6413,7 @@
       </c>
       <c r="K3" s="23">
         <f>IF(COUNTIF(درصد!B$2:B$44,C3)&gt;0, INDEX(درصد!I$2:I$44,MATCH(C3,درصد!B$2:B$44,0)),0)</f>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="L3" s="23">
         <f>IF(COUNTIF(درصد!B$2:B$44,C3)&gt;0, INDEX(درصد!J$2:J$44,MATCH(C3,درصد!B$2:B$44,0)),0)</f>
@@ -6429,13 +6429,13 @@
       </c>
       <c r="O3" s="26">
         <f>IF(COUNTIF(درصد!B$2:B$44,C3)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C3,درصد!B$2:B$44,0)),0)</f>
-        <v>73.333333333333329</v>
+        <v>86.666666666666671</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18.600000000000001" x14ac:dyDescent="0.6">
       <c r="A4" s="24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="28" t="s">
         <v>61</v>
@@ -9010,7 +9010,7 @@
       </c>
       <c r="C9" s="41">
         <f>IF(COUNTIF(درصد!B$2:B$44,B9)&gt;0, INDEX(درصد!M$2:M$44,MATCH(B9,درصد!B$2:B$44,0)),0)</f>
-        <v>73.333333333333329</v>
+        <v>86.666666666666671</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -9419,8 +9419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="O44" sqref="A1:O44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:O44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -9480,10 +9480,10 @@
         <f>RANK(O2, O$2:O$42)</f>
         <v>1</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="56">
+      <c r="C2" s="53">
         <v>1011</v>
       </c>
       <c r="D2" s="23" t="str">
@@ -9530,7 +9530,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C2)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C2,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O2" s="57">
+      <c r="O2" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C2)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C2,درصد!B$2:B$44,0)),0)</f>
         <v>100</v>
       </c>
@@ -9540,10 +9540,10 @@
         <f t="shared" ref="A3:A42" si="0">RANK(O3, O$2:O$42)</f>
         <v>2</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="56">
+      <c r="C3" s="53">
         <v>1026</v>
       </c>
       <c r="D3" s="23" t="str">
@@ -9590,7 +9590,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C3)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C3,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O3" s="57">
+      <c r="O3" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C3)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C3,درصد!B$2:B$44,0)),0)</f>
         <v>86.666666666666671</v>
       </c>
@@ -9598,12 +9598,12 @@
     <row r="4" spans="1:15" ht="18.600000000000001" x14ac:dyDescent="0.6">
       <c r="A4" s="24">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B4" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="52" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="56">
+      <c r="C4" s="53">
         <v>1008</v>
       </c>
       <c r="D4" s="23" t="str">
@@ -9636,7 +9636,7 @@
       </c>
       <c r="K4" s="23">
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C4)&gt;0, INDEX(گوگل!I$2:I$44,MATCH($C4,گوگل!$B$2:$B$44,0)),0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="23">
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C4)&gt;0, INDEX(گوگل!J$2:J$44,MATCH($C4,گوگل!$B$2:$B$44,0)),0)</f>
@@ -9650,20 +9650,20 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C4)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C4,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O4" s="57">
+      <c r="O4" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C4)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C4,درصد!B$2:B$44,0)),0)</f>
-        <v>73.333333333333329</v>
+        <v>86.666666666666671</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="18.600000000000001" x14ac:dyDescent="0.6">
       <c r="A5" s="24">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="B5" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="56">
+      <c r="C5" s="53">
         <v>1015</v>
       </c>
       <c r="D5" s="23" t="str">
@@ -9710,7 +9710,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C5)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C5,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O5" s="57">
+      <c r="O5" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C5)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C5,درصد!B$2:B$44,0)),0)</f>
         <v>73.333333333333329</v>
       </c>
@@ -9720,10 +9720,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="56">
+      <c r="C6" s="53">
         <v>1031</v>
       </c>
       <c r="D6" s="23" t="str">
@@ -9770,7 +9770,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C6)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C6,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O6" s="57">
+      <c r="O6" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C6)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C6,درصد!B$2:B$44,0)),0)</f>
         <v>70</v>
       </c>
@@ -9780,10 +9780,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="55" t="s">
+      <c r="B7" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="56">
+      <c r="C7" s="53">
         <v>1016</v>
       </c>
       <c r="D7" s="23" t="str">
@@ -9830,7 +9830,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C7)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C7,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O7" s="57">
+      <c r="O7" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C7)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C7,درصد!B$2:B$44,0)),0)</f>
         <v>66.666666666666657</v>
       </c>
@@ -9840,10 +9840,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="55" t="s">
+      <c r="B8" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="56">
+      <c r="C8" s="53">
         <v>1006</v>
       </c>
       <c r="D8" s="23" t="str">
@@ -9890,7 +9890,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C8)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C8,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O8" s="57">
+      <c r="O8" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C8)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C8,درصد!B$2:B$44,0)),0)</f>
         <v>63.333333333333329</v>
       </c>
@@ -9900,10 +9900,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="53">
         <v>1041</v>
       </c>
       <c r="D9" s="23" t="str">
@@ -9950,7 +9950,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C9)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C9,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O9" s="57">
+      <c r="O9" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C9)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C9,درصد!B$2:B$44,0)),0)</f>
         <v>53.333333333333336</v>
       </c>
@@ -9960,10 +9960,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="56">
+      <c r="C10" s="53">
         <v>1022</v>
       </c>
       <c r="D10" s="23" t="str">
@@ -10010,7 +10010,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C10)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C10,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O10" s="57">
+      <c r="O10" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C10)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C10,درصد!B$2:B$44,0)),0)</f>
         <v>53.333333333333336</v>
       </c>
@@ -10020,10 +10020,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="55" t="s">
+      <c r="B11" s="52" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="56">
+      <c r="C11" s="53">
         <v>1039</v>
       </c>
       <c r="D11" s="23" t="str">
@@ -10070,7 +10070,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C11)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C11,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O11" s="57">
+      <c r="O11" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C11)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C11,درصد!B$2:B$44,0)),0)</f>
         <v>50</v>
       </c>
@@ -10080,10 +10080,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B12" s="55" t="s">
+      <c r="B12" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="56">
+      <c r="C12" s="53">
         <v>1005</v>
       </c>
       <c r="D12" s="23" t="str">
@@ -10130,7 +10130,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C12)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C12,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O12" s="57">
+      <c r="O12" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C12)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C12,درصد!B$2:B$44,0)),0)</f>
         <v>50</v>
       </c>
@@ -10140,10 +10140,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="56">
+      <c r="C13" s="53">
         <v>1017</v>
       </c>
       <c r="D13" s="23" t="str">
@@ -10190,7 +10190,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C13)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C13,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O13" s="57">
+      <c r="O13" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C13)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C13,درصد!B$2:B$44,0)),0)</f>
         <v>50</v>
       </c>
@@ -10200,10 +10200,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B14" s="55" t="s">
+      <c r="B14" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="56">
+      <c r="C14" s="53">
         <v>1010</v>
       </c>
       <c r="D14" s="23" t="str">
@@ -10250,7 +10250,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C14)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C14,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O14" s="57">
+      <c r="O14" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C14)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C14,درصد!B$2:B$44,0)),0)</f>
         <v>50</v>
       </c>
@@ -10260,10 +10260,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B15" s="55" t="s">
+      <c r="B15" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="56">
+      <c r="C15" s="53">
         <v>1003</v>
       </c>
       <c r="D15" s="23" t="str">
@@ -10310,7 +10310,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C15)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C15,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O15" s="57">
+      <c r="O15" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C15)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C15,درصد!B$2:B$44,0)),0)</f>
         <v>50</v>
       </c>
@@ -10320,10 +10320,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="55" t="s">
+      <c r="B16" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="56">
+      <c r="C16" s="53">
         <v>1020</v>
       </c>
       <c r="D16" s="23" t="str">
@@ -10370,7 +10370,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C16)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C16,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O16" s="57">
+      <c r="O16" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C16)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C16,درصد!B$2:B$44,0)),0)</f>
         <v>43.333333333333336</v>
       </c>
@@ -10380,10 +10380,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="55" t="s">
+      <c r="B17" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="56">
+      <c r="C17" s="53">
         <v>1014</v>
       </c>
       <c r="D17" s="23" t="str">
@@ -10430,7 +10430,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C17)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C17,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O17" s="57">
+      <c r="O17" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C17)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C17,درصد!B$2:B$44,0)),0)</f>
         <v>40</v>
       </c>
@@ -10440,10 +10440,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B18" s="55" t="s">
+      <c r="B18" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="56">
+      <c r="C18" s="53">
         <v>1036</v>
       </c>
       <c r="D18" s="23" t="str">
@@ -10490,7 +10490,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C18)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C18,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O18" s="57">
+      <c r="O18" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C18)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C18,درصد!B$2:B$44,0)),0)</f>
         <v>40</v>
       </c>
@@ -10500,10 +10500,10 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="55" t="s">
+      <c r="B19" s="52" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="53">
         <v>1021</v>
       </c>
       <c r="D19" s="23" t="str">
@@ -10550,7 +10550,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C19)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C19,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O19" s="57">
+      <c r="O19" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C19)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C19,درصد!B$2:B$44,0)),0)</f>
         <v>36.666666666666664</v>
       </c>
@@ -10560,10 +10560,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="53">
         <v>1025</v>
       </c>
       <c r="D20" s="23" t="str">
@@ -10610,7 +10610,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C20)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C20,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O20" s="57">
+      <c r="O20" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C20)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C20,درصد!B$2:B$44,0)),0)</f>
         <v>33.333333333333329</v>
       </c>
@@ -10620,10 +10620,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B21" s="55" t="s">
+      <c r="B21" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="53">
         <v>1040</v>
       </c>
       <c r="D21" s="23" t="str">
@@ -10670,7 +10670,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C21)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C21,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O21" s="57">
+      <c r="O21" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C21)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C21,درصد!B$2:B$44,0)),0)</f>
         <v>33.333333333333329</v>
       </c>
@@ -10680,10 +10680,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="56">
+      <c r="C22" s="53">
         <v>1038</v>
       </c>
       <c r="D22" s="23" t="str">
@@ -10730,7 +10730,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C22)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C22,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O22" s="57">
+      <c r="O22" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C22)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C22,درصد!B$2:B$44,0)),0)</f>
         <v>33.333333333333329</v>
       </c>
@@ -10740,10 +10740,10 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="55" t="s">
+      <c r="B23" s="52" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="56">
+      <c r="C23" s="53">
         <v>1009</v>
       </c>
       <c r="D23" s="23" t="str">
@@ -10790,7 +10790,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C23)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C23,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O23" s="57">
+      <c r="O23" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C23)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C23,درصد!B$2:B$44,0)),0)</f>
         <v>30</v>
       </c>
@@ -10800,10 +10800,10 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="56">
+      <c r="C24" s="53">
         <v>1007</v>
       </c>
       <c r="D24" s="23" t="str">
@@ -10850,7 +10850,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C24)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C24,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O24" s="57">
+      <c r="O24" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C24)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C24,درصد!B$2:B$44,0)),0)</f>
         <v>30</v>
       </c>
@@ -10860,10 +10860,10 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B25" s="55" t="s">
+      <c r="B25" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="56">
+      <c r="C25" s="53">
         <v>1034</v>
       </c>
       <c r="D25" s="23" t="str">
@@ -10910,7 +10910,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C25)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C25,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O25" s="57">
+      <c r="O25" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C25)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C25,درصد!B$2:B$44,0)),0)</f>
         <v>30</v>
       </c>
@@ -10920,10 +10920,10 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="56">
+      <c r="C26" s="53">
         <v>1018</v>
       </c>
       <c r="D26" s="23" t="str">
@@ -10970,7 +10970,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C26)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C26,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O26" s="57">
+      <c r="O26" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C26)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C26,درصد!B$2:B$44,0)),0)</f>
         <v>26.666666666666668</v>
       </c>
@@ -10980,10 +10980,10 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="C27" s="56">
+      <c r="C27" s="53">
         <v>1028</v>
       </c>
       <c r="D27" s="23" t="str">
@@ -11030,7 +11030,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C27)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C27,گوگل!$B$2:$B$44,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="O27" s="57">
+      <c r="O27" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C27)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C27,درصد!B$2:B$44,0)),0)</f>
         <v>23.333333333333332</v>
       </c>
@@ -11040,10 +11040,10 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="56">
+      <c r="C28" s="53">
         <v>1024</v>
       </c>
       <c r="D28" s="23" t="str">
@@ -11090,7 +11090,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C28)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C28,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O28" s="57">
+      <c r="O28" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C28)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C28,درصد!B$2:B$44,0)),0)</f>
         <v>20</v>
       </c>
@@ -11100,10 +11100,10 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="C29" s="56">
+      <c r="C29" s="53">
         <v>1030</v>
       </c>
       <c r="D29" s="23" t="str">
@@ -11150,7 +11150,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C29)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C29,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O29" s="57">
+      <c r="O29" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C29)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C29,درصد!B$2:B$44,0)),0)</f>
         <v>20</v>
       </c>
@@ -11160,10 +11160,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="55" t="s">
+      <c r="B30" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C30" s="56">
+      <c r="C30" s="53">
         <v>1037</v>
       </c>
       <c r="D30" s="23" t="str">
@@ -11210,7 +11210,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C30)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C30,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O30" s="57">
+      <c r="O30" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C30)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C30,درصد!B$2:B$44,0)),0)</f>
         <v>16.666666666666664</v>
       </c>
@@ -11220,10 +11220,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B31" s="55" t="s">
+      <c r="B31" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="56">
+      <c r="C31" s="53">
         <v>1001</v>
       </c>
       <c r="D31" s="23" t="str">
@@ -11270,7 +11270,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C31)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C31,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O31" s="57">
+      <c r="O31" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C31)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C31,درصد!B$2:B$44,0)),0)</f>
         <v>16.666666666666664</v>
       </c>
@@ -11280,10 +11280,10 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="56">
+      <c r="C32" s="53">
         <v>1004</v>
       </c>
       <c r="D32" s="23" t="str">
@@ -11330,7 +11330,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C32)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C32,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O32" s="57">
+      <c r="O32" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C32)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C32,درصد!B$2:B$44,0)),0)</f>
         <v>6.666666666666667</v>
       </c>
@@ -11340,10 +11340,10 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B33" s="55" t="s">
+      <c r="B33" s="52" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="56">
+      <c r="C33" s="53">
         <v>1035</v>
       </c>
       <c r="D33" s="23" t="str">
@@ -11390,7 +11390,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C33)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C33,گوگل!$B$2:$B$44,0)),0)</f>
         <v>2</v>
       </c>
-      <c r="O33" s="57">
+      <c r="O33" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C33)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C33,درصد!B$2:B$44,0)),0)</f>
         <v>6.666666666666667</v>
       </c>
@@ -11400,10 +11400,10 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="55" t="s">
+      <c r="B34" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="C34" s="56">
+      <c r="C34" s="53">
         <v>1029</v>
       </c>
       <c r="D34" s="23" t="str">
@@ -11450,7 +11450,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C34)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C34,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O34" s="57">
+      <c r="O34" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C34)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C34,درصد!B$2:B$44,0)),0)</f>
         <v>3.3333333333333335</v>
       </c>
@@ -11460,10 +11460,10 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B35" s="55" t="s">
+      <c r="B35" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="56">
+      <c r="C35" s="53">
         <v>1033</v>
       </c>
       <c r="D35" s="23" t="str">
@@ -11510,7 +11510,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C35)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C35,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O35" s="57">
+      <c r="O35" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C35)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C35,درصد!B$2:B$44,0)),0)</f>
         <v>3.3333333333333335</v>
       </c>
@@ -11520,10 +11520,10 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="55" t="s">
+      <c r="B36" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="56">
+      <c r="C36" s="53">
         <v>1012</v>
       </c>
       <c r="D36" s="23" t="str">
@@ -11570,7 +11570,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C36)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C36,گوگل!$B$2:$B$44,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="O36" s="57">
+      <c r="O36" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C36)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C36,درصد!B$2:B$44,0)),0)</f>
         <v>0</v>
       </c>
@@ -11580,10 +11580,10 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B37" s="55" t="s">
+      <c r="B37" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="56">
+      <c r="C37" s="53">
         <v>1023</v>
       </c>
       <c r="D37" s="23" t="str">
@@ -11630,7 +11630,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C37)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C37,گوگل!$B$2:$B$44,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="O37" s="57">
+      <c r="O37" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C37)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C37,درصد!B$2:B$44,0)),0)</f>
         <v>0</v>
       </c>
@@ -11640,10 +11640,10 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B38" s="55" t="s">
+      <c r="B38" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="56">
+      <c r="C38" s="53">
         <v>1019</v>
       </c>
       <c r="D38" s="23" t="str">
@@ -11690,7 +11690,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C38)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C38,گوگل!$B$2:$B$44,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="O38" s="57">
+      <c r="O38" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C38)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C38,درصد!B$2:B$44,0)),0)</f>
         <v>0</v>
       </c>
@@ -11700,10 +11700,10 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B39" s="55" t="s">
+      <c r="B39" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="C39" s="56">
+      <c r="C39" s="53">
         <v>1032</v>
       </c>
       <c r="D39" s="23" t="str">
@@ -11750,7 +11750,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C39)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C39,گوگل!$B$2:$B$44,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="O39" s="57">
+      <c r="O39" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C39)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C39,درصد!B$2:B$44,0)),0)</f>
         <v>0</v>
       </c>
@@ -11760,10 +11760,10 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="55" t="s">
+      <c r="B40" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="56">
+      <c r="C40" s="53">
         <v>1013</v>
       </c>
       <c r="D40" s="23" t="str">
@@ -11810,7 +11810,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C40)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C40,گوگل!$B$2:$B$44,0)),0)</f>
         <v>4</v>
       </c>
-      <c r="O40" s="57">
+      <c r="O40" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C40)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C40,درصد!B$2:B$44,0)),0)</f>
         <v>-3.3333333333333335</v>
       </c>
@@ -11820,10 +11820,10 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="56">
+      <c r="C41" s="53">
         <v>1027</v>
       </c>
       <c r="D41" s="23" t="str">
@@ -11870,7 +11870,7 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C41)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C41,گوگل!$B$2:$B$44,0)),0)</f>
         <v>0</v>
       </c>
-      <c r="O41" s="57">
+      <c r="O41" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C41)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C41,درصد!B$2:B$44,0)),0)</f>
         <v>-3.3333333333333335</v>
       </c>
@@ -11880,10 +11880,10 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="55" t="s">
+      <c r="B42" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="56">
+      <c r="C42" s="53">
         <v>1002</v>
       </c>
       <c r="D42" s="23" t="str">
@@ -11930,27 +11930,27 @@
         <f>IF(COUNTIF(گوگل!$B$2:$B$44,$C42)&gt;0, INDEX(گوگل!L$2:L$44,MATCH($C42,گوگل!$B$2:$B$44,0)),0)</f>
         <v>3</v>
       </c>
-      <c r="O42" s="57">
+      <c r="O42" s="54">
         <f>IF(COUNTIF(درصد!B$2:B$44,C42)&gt;0, INDEX(درصد!M$2:M$44,MATCH(C42,درصد!B$2:B$44,0)),0)</f>
         <v>-6.666666666666667</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="16.8" x14ac:dyDescent="0.5">
-      <c r="A43" s="53"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="54"/>
-      <c r="D43" s="54"/>
-      <c r="E43" s="54"/>
-      <c r="F43" s="54"/>
-      <c r="G43" s="54"/>
-      <c r="H43" s="54"/>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
-      <c r="K43" s="54"/>
-      <c r="L43" s="54"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="54"/>
-      <c r="O43" s="54"/>
+      <c r="A43" s="50"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="51"/>
+      <c r="H43" s="51"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
+      <c r="K43" s="51"/>
+      <c r="L43" s="51"/>
+      <c r="M43" s="51"/>
+      <c r="N43" s="51"/>
+      <c r="O43" s="51"/>
     </row>
     <row r="44" spans="1:15" ht="18.600000000000001" x14ac:dyDescent="0.6">
       <c r="A44" s="49" t="s">

</xml_diff>